<commit_message>
fix: 0.20.48-beta bug fixing TPN
</commit_message>
<xml_diff>
--- a/db/GlobParEnt.xlsx
+++ b/db/GlobParEnt.xlsx
@@ -117,18 +117,9 @@
     <t>KCl 7,4%</t>
   </si>
   <si>
-    <t>CaCl2</t>
-  </si>
-  <si>
     <t>CaGluc 10%</t>
   </si>
   <si>
-    <t>MgCl2</t>
-  </si>
-  <si>
-    <t>MgCl 10%</t>
-  </si>
-  <si>
     <t>KNaFosfaat</t>
   </si>
   <si>
@@ -232,6 +223,15 @@
   </si>
   <si>
     <t>BAXA bereiding</t>
+  </si>
+  <si>
+    <t>CaCl2 3,3%</t>
+  </si>
+  <si>
+    <t>MgCl2 10%</t>
+  </si>
+  <si>
+    <t>MgSulfaat</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -632,81 +632,81 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>57</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>58</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>59</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>60</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>61</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>62</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>63</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" t="s">
-        <v>70</v>
-      </c>
       <c r="M4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1.8E-3</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0.22500000000000001</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1726,12 +1726,12 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0.5</v>
+        <v>0.64</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1808,12 +1808,12 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1893,18 +1893,18 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>0.28999999999999998</v>
       </c>
       <c r="C33">
-        <v>7.4285714285714302E-2</v>
+        <v>7.4300000000000005E-2</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1913,19 +1913,19 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>5.4285714285714298E-2</v>
+        <v>5.4300000000000001E-2</v>
       </c>
       <c r="G33">
-        <v>7.1428571428571397E-2</v>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="H33">
-        <v>2.57142857142857E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="I33">
-        <v>3.4285714285714301E-2</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="J33">
-        <v>4.2857142857142903E-3</v>
+        <v>4.2900000000000004E-3</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1939,13 +1939,13 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>0.28999999999999998</v>
       </c>
       <c r="C34">
-        <v>7.4285714285714302E-2</v>
+        <v>7.4300000000000005E-2</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1954,19 +1954,19 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>7.14285714285714E-3</v>
+        <v>7.1399999999999996E-3</v>
       </c>
       <c r="G34">
-        <v>1.7142857142857099E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="H34">
-        <v>2.57142857142857E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="I34">
-        <v>2.1428571428571401E-2</v>
+        <v>2.1399999999999999E-2</v>
       </c>
       <c r="J34">
-        <v>5.7142857142857099E-3</v>
+        <v>5.7099999999999998E-3</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <v>0.32</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>0.35</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>0.33</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>0.96</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>1.8</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44">
         <v>1.8</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <v>1.8</v>
@@ -2431,6 +2431,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: 0.20.54-beta pediatrie (bijna) gefikst
</commit_message>
<xml_diff>
--- a/db/GlobParEnt.xlsx
+++ b/db/GlobParEnt.xlsx
@@ -30,9 +30,6 @@
     <t>GLUCOSE 10 % FREEFLEX INFUSIEZAK 500 ML</t>
   </si>
   <si>
-    <t>glucose 12,5 %</t>
-  </si>
-  <si>
     <t>glucose 15%</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>MgSulfaat</t>
+  </si>
+  <si>
+    <t>glucose 12,5%</t>
   </si>
 </sst>
 </file>
@@ -573,9 +573,7 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -586,7 +584,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -632,81 +630,81 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>57</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>58</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>59</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>60</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>61</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>62</v>
-      </c>
-      <c r="N3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
         <v>66</v>
       </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -799,7 +797,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -838,12 +836,12 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0.6</v>
@@ -882,12 +880,12 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0.7</v>
@@ -928,7 +926,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>0.8</v>
@@ -967,12 +965,12 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1011,12 +1009,12 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1.2</v>
@@ -1055,12 +1053,12 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>1.4</v>
@@ -1099,12 +1097,12 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>1.6</v>
@@ -1143,12 +1141,12 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1.8</v>
@@ -1187,12 +1185,12 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -1231,12 +1229,12 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>0.2</v>
@@ -1277,7 +1275,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>0.2</v>
@@ -1318,7 +1316,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1359,7 +1357,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1398,12 +1396,12 @@
         <v>0.155</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1444,7 +1442,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1485,7 +1483,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1526,7 +1524,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1567,7 +1565,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1608,7 +1606,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1649,7 +1647,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1690,7 +1688,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1731,7 +1729,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1772,7 +1770,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1813,7 +1811,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1854,7 +1852,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1893,12 +1891,12 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>0.28999999999999998</v>
@@ -1939,7 +1937,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>0.28999999999999998</v>
@@ -1980,7 +1978,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>0.32</v>
@@ -2021,7 +2019,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>0.35</v>
@@ -2062,7 +2060,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>0.33</v>
@@ -2103,7 +2101,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>0.96</v>
@@ -2144,7 +2142,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2185,7 +2183,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2226,7 +2224,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -2267,7 +2265,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -2308,7 +2306,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>1.8</v>
@@ -2349,7 +2347,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>1.8</v>
@@ -2390,7 +2388,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>1.8</v>

</xml_diff>

<commit_message>
tests: TPN test scenarios toegevoegd
</commit_message>
<xml_diff>
--- a/db/GlobParEnt.xlsx
+++ b/db/GlobParEnt.xlsx
@@ -573,7 +573,9 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1249,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>7.6999999999999999E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1270,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>7.6999999999999999E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1724,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>0.45200000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -1902,7 +1904,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="C33">
-        <v>7.4300000000000005E-2</v>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1932,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -1940,7 +1942,7 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="C34">
         <v>7.4300000000000005E-2</v>
@@ -1973,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>6.2899999999999998E-2</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2014,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2055,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2096,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2380,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <v>0</v>
+        <v>6.67</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -2421,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="L45">
-        <v>0</v>
+        <v>6.67</v>
       </c>
       <c r="M45">
         <v>0</v>

</xml_diff>

<commit_message>
feat: completed impl of config for ped/neo and parent
</commit_message>
<xml_diff>
--- a/db/GlobParEnt.xlsx
+++ b/db/GlobParEnt.xlsx
@@ -11,7 +11,10 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="Tbl_Admin_ParEnt">Tbl_Admin_ParEnt!$A$6:$N$47</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -577,7 +580,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="A6" sqref="A6:N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>